<commit_message>
🔄 Sync automática - 23/06/2025 08:00
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\CotizadorKitchenTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C934B165-BB09-4FBA-8E3F-84E6F593AA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECC858E4-B144-424C-BC6B-910E707153B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F61FC40-0691-40CF-AA3F-A57196392FE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C258EBDA-F0AD-42A6-BA63-8F24592EF026}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Precio" sheetId="1" r:id="rId1"/>
@@ -16214,11 +16214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58086886-AB9F-49FF-9680-94FE052267EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654C190F-4407-4359-A7F1-D681214AF078}">
   <dimension ref="A1:C5267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A5224" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
🔄 Actualización automática 2025-06-25 16:07:31
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\CotizadorKitchenTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECC858E4-B144-424C-BC6B-910E707153B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{274D6944-72EA-41A0-9902-8CE054785788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C258EBDA-F0AD-42A6-BA63-8F24592EF026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{070DD0CD-9BD5-43D3-82E6-24815C2543FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Precio" sheetId="1" r:id="rId1"/>
@@ -14438,16 +14438,16 @@
     <t>TAPA VIDRIO 20 CM (103082)</t>
   </si>
   <si>
-    <t>TAPA VIDRIO 22 CM (103083)</t>
+    <t>TAPA VIDRIO 22 CM (16948)</t>
   </si>
   <si>
     <t>TAPA VIDRIO 24 CM (103084)</t>
   </si>
   <si>
-    <t>TAPA VIDRIO 26 CM (103085)</t>
-  </si>
-  <si>
-    <t>TAPA VIDRIO 28 CM (103080)</t>
+    <t>TAPA VIDRIO 26 CM (16950)</t>
+  </si>
+  <si>
+    <t>TAPA VIDRIO 28 CM (103080 | 16951)</t>
   </si>
   <si>
     <t>TAPON A PALANCA (BTER. X1) NEGRO LM. (575)</t>
@@ -15837,15 +15837,18 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -16214,11 +16217,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654C190F-4407-4359-A7F1-D681214AF078}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFD0963-C3A6-4E24-B11B-26D5EB0218AC}">
   <dimension ref="A1:C5267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5224" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5267"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -63561,7 +63564,7 @@
         <v>4300</v>
       </c>
       <c r="C4305" s="3">
-        <v>39124.800000000003</v>
+        <v>37135.214999999997</v>
       </c>
     </row>
     <row r="4306" spans="1:3" x14ac:dyDescent="0.2">
@@ -64056,7 +64059,7 @@
         <v>4344</v>
       </c>
       <c r="C4350" s="3">
-        <v>62004.6</v>
+        <v>56692.485000000001</v>
       </c>
     </row>
     <row r="4351" spans="1:3" x14ac:dyDescent="0.2">
@@ -64067,7 +64070,7 @@
         <v>4345</v>
       </c>
       <c r="C4351" s="3">
-        <v>27473.715</v>
+        <v>26020.215</v>
       </c>
     </row>
     <row r="4352" spans="1:3" x14ac:dyDescent="0.2">
@@ -66795,7 +66798,7 @@
         <v>4593</v>
       </c>
       <c r="C4599" s="3">
-        <v>56954.97</v>
+        <v>55403.144999999997</v>
       </c>
     </row>
     <row r="4600" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
🔄 Actualización automática 2025-07-01 08:49:10
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\CotizadorKitchenTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{274D6944-72EA-41A0-9902-8CE054785788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D87EC7E4-F392-408E-A145-61F6596A0CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{070DD0CD-9BD5-43D3-82E6-24815C2543FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46639BCD-CEDA-4172-918A-23A2AB4D2D26}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Precio" sheetId="1" r:id="rId1"/>
@@ -7265,9 +7265,6 @@
     <t>JARRO MUG MELAM. BLANCA CONICO 390 CC (66744)</t>
   </si>
   <si>
-    <t>JARRO MUG MELAM. BLANCA RECTO 350 CC (8184)</t>
-  </si>
-  <si>
     <t>JARRO MUG MELAM. DEC PIEDRAS MULTICOLOR 9" (68063)</t>
   </si>
   <si>
@@ -7275,6 +7272,9 @@
   </si>
   <si>
     <t>JARRO MUG MELAM. DEC. ROCOCO 9" (67398)</t>
+  </si>
+  <si>
+    <t>JARRO MUG MELAM. RECTO 350 CC (8184)</t>
   </si>
   <si>
     <t>JARRO MUG MELAMINA 350 CC X6 (66744)</t>
@@ -15837,18 +15837,15 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -16217,11 +16214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFD0963-C3A6-4E24-B11B-26D5EB0218AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B03AEB3-6D12-4964-B554-A11408A99C55}">
   <dimension ref="A1:C5267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A5224" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18981,7 +18978,7 @@
         <v>252</v>
       </c>
       <c r="C252" s="3">
-        <v>18120.014999999999</v>
+        <v>19026.015749999999</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
@@ -18992,7 +18989,7 @@
         <v>253</v>
       </c>
       <c r="C253" s="3">
-        <v>18709.965</v>
+        <v>19645.463250000001</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
@@ -19003,7 +19000,7 @@
         <v>254</v>
       </c>
       <c r="C254" s="3">
-        <v>19234.080000000002</v>
+        <v>20195.784</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
@@ -19014,7 +19011,7 @@
         <v>255</v>
       </c>
       <c r="C255" s="3">
-        <v>20675.61</v>
+        <v>21709.390500000001</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
@@ -19025,7 +19022,7 @@
         <v>256</v>
       </c>
       <c r="C256" s="3">
-        <v>21199.724999999999</v>
+        <v>22259.71125</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
@@ -19036,7 +19033,7 @@
         <v>257</v>
       </c>
       <c r="C257" s="3">
-        <v>21854.654999999999</v>
+        <v>22947.387750000002</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
@@ -23370,7 +23367,7 @@
         <v>651</v>
       </c>
       <c r="C651" s="3">
-        <v>62650.125</v>
+        <v>65782.631250000006</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.2">
@@ -23381,7 +23378,7 @@
         <v>652</v>
       </c>
       <c r="C652" s="3">
-        <v>69555.960000000006</v>
+        <v>73033.758000000002</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.2">
@@ -23392,7 +23389,7 @@
         <v>653</v>
       </c>
       <c r="C653" s="3">
-        <v>51252.974999999999</v>
+        <v>53815.623749999999</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.2">
@@ -23403,7 +23400,7 @@
         <v>654</v>
       </c>
       <c r="C654" s="3">
-        <v>55216.754999999997</v>
+        <v>57977.592750000003</v>
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.2">
@@ -23414,7 +23411,7 @@
         <v>655</v>
       </c>
       <c r="C655" s="3">
-        <v>60117.614999999998</v>
+        <v>63123.495750000002</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.2">
@@ -23425,7 +23422,7 @@
         <v>656</v>
       </c>
       <c r="C656" s="3">
-        <v>61991.775000000001</v>
+        <v>65091.363749999997</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.2">
@@ -23436,7 +23433,7 @@
         <v>657</v>
       </c>
       <c r="C657" s="3">
-        <v>64730.34</v>
+        <v>67966.857000000004</v>
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.2">
@@ -23447,7 +23444,7 @@
         <v>658</v>
       </c>
       <c r="C658" s="3">
-        <v>67757.039999999994</v>
+        <v>71144.892000000007</v>
       </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.2">
@@ -23480,7 +23477,7 @@
         <v>661</v>
       </c>
       <c r="C661" s="3">
-        <v>71380.53</v>
+        <v>74949.556500000006</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.2">
@@ -23491,7 +23488,7 @@
         <v>662</v>
       </c>
       <c r="C662" s="3">
-        <v>75746.16</v>
+        <v>79533.467999999993</v>
       </c>
     </row>
     <row r="663" spans="1:3" x14ac:dyDescent="0.2">
@@ -32786,7 +32783,7 @@
         <v>1507</v>
       </c>
       <c r="C1507" s="3">
-        <v>19633.365000000002</v>
+        <v>20615.03325</v>
       </c>
     </row>
     <row r="1508" spans="1:3" x14ac:dyDescent="0.2">
@@ -32797,7 +32794,7 @@
         <v>1508</v>
       </c>
       <c r="C1508" s="3">
-        <v>20282.310000000001</v>
+        <v>21296.425500000001</v>
       </c>
     </row>
     <row r="1509" spans="1:3" x14ac:dyDescent="0.2">
@@ -32808,7 +32805,7 @@
         <v>1509</v>
       </c>
       <c r="C1509" s="3">
-        <v>21003.075000000001</v>
+        <v>22053.228749999998</v>
       </c>
     </row>
     <row r="1510" spans="1:3" x14ac:dyDescent="0.2">
@@ -32819,7 +32816,7 @@
         <v>1510</v>
       </c>
       <c r="C1510" s="3">
-        <v>22444.605</v>
+        <v>23566.83525</v>
       </c>
     </row>
     <row r="1511" spans="1:3" x14ac:dyDescent="0.2">
@@ -32830,7 +32827,7 @@
         <v>1511</v>
       </c>
       <c r="C1511" s="3">
-        <v>23741.64</v>
+        <v>24928.722000000002</v>
       </c>
     </row>
     <row r="1512" spans="1:3" x14ac:dyDescent="0.2">
@@ -32841,7 +32838,7 @@
         <v>1512</v>
       </c>
       <c r="C1512" s="3">
-        <v>25471.305</v>
+        <v>26744.87025</v>
       </c>
     </row>
     <row r="1513" spans="1:3" x14ac:dyDescent="0.2">
@@ -32852,7 +32849,7 @@
         <v>1513</v>
       </c>
       <c r="C1513" s="3">
-        <v>18507.330000000002</v>
+        <v>19432.696499999998</v>
       </c>
     </row>
     <row r="1514" spans="1:3" x14ac:dyDescent="0.2">
@@ -32863,7 +32860,7 @@
         <v>1514</v>
       </c>
       <c r="C1514" s="3">
-        <v>18552.645</v>
+        <v>19480.277249999999</v>
       </c>
     </row>
     <row r="1515" spans="1:3" x14ac:dyDescent="0.2">
@@ -32874,7 +32871,7 @@
         <v>1515</v>
       </c>
       <c r="C1515" s="3">
-        <v>19162.259999999998</v>
+        <v>20120.373</v>
       </c>
     </row>
     <row r="1516" spans="1:3" x14ac:dyDescent="0.2">
@@ -32885,7 +32882,7 @@
         <v>1516</v>
       </c>
       <c r="C1516" s="3">
-        <v>20497.77</v>
+        <v>21522.658500000001</v>
       </c>
     </row>
     <row r="1517" spans="1:3" x14ac:dyDescent="0.2">
@@ -34645,7 +34642,7 @@
         <v>1676</v>
       </c>
       <c r="C1676" s="3">
-        <v>1449271.17</v>
+        <v>1492730.82</v>
       </c>
     </row>
     <row r="1677" spans="1:3" x14ac:dyDescent="0.2">
@@ -37010,7 +37007,7 @@
         <v>1891</v>
       </c>
       <c r="C1891" s="3">
-        <v>2620368.09</v>
+        <v>2646048.0150000001</v>
       </c>
     </row>
     <row r="1892" spans="1:3" x14ac:dyDescent="0.2">
@@ -37098,7 +37095,7 @@
         <v>1899</v>
       </c>
       <c r="C1899" s="3">
-        <v>1468197.45</v>
+        <v>1512232.5149999999</v>
       </c>
     </row>
     <row r="1900" spans="1:3" x14ac:dyDescent="0.2">
@@ -42713,29 +42710,29 @@
     </row>
     <row r="2410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2410" s="5">
-        <v>1143969</v>
+        <v>1143735</v>
       </c>
       <c r="B2410" s="4" t="s">
         <v>2410</v>
       </c>
       <c r="C2410" s="3">
-        <v>5045.3549999999996</v>
+        <v>4313.4750000000004</v>
       </c>
     </row>
     <row r="2411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2411" s="5">
-        <v>1143735</v>
+        <v>1143725</v>
       </c>
       <c r="B2411" s="4" t="s">
         <v>2411</v>
       </c>
       <c r="C2411" s="3">
-        <v>4313.4750000000004</v>
+        <v>4434.03</v>
       </c>
     </row>
     <row r="2412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2412" s="5">
-        <v>1143725</v>
+        <v>1143716</v>
       </c>
       <c r="B2412" s="4" t="s">
         <v>2412</v>
@@ -42746,13 +42743,13 @@
     </row>
     <row r="2413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2413" s="5">
-        <v>1143716</v>
+        <v>1143969</v>
       </c>
       <c r="B2413" s="4" t="s">
         <v>2413</v>
       </c>
       <c r="C2413" s="3">
-        <v>4434.03</v>
+        <v>5045.3549999999996</v>
       </c>
     </row>
     <row r="2414" spans="1:3" x14ac:dyDescent="0.2">
@@ -43038,7 +43035,7 @@
         <v>2439</v>
       </c>
       <c r="C2439" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2440" spans="1:3" x14ac:dyDescent="0.2">
@@ -43049,7 +43046,7 @@
         <v>2440</v>
       </c>
       <c r="C2440" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2441" spans="1:3" x14ac:dyDescent="0.2">
@@ -43060,7 +43057,7 @@
         <v>2441</v>
       </c>
       <c r="C2441" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2442" spans="1:3" x14ac:dyDescent="0.2">
@@ -43071,7 +43068,7 @@
         <v>2442</v>
       </c>
       <c r="C2442" s="3">
-        <v>0</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2443" spans="1:3" x14ac:dyDescent="0.2">
@@ -43082,7 +43079,7 @@
         <v>2443</v>
       </c>
       <c r="C2443" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2444" spans="1:3" x14ac:dyDescent="0.2">
@@ -43093,7 +43090,7 @@
         <v>2444</v>
       </c>
       <c r="C2444" s="3">
-        <v>0</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2445" spans="1:3" x14ac:dyDescent="0.2">
@@ -43104,7 +43101,7 @@
         <v>2445</v>
       </c>
       <c r="C2445" s="3">
-        <v>28692.09</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2446" spans="1:3" x14ac:dyDescent="0.2">
@@ -43115,7 +43112,7 @@
         <v>2446</v>
       </c>
       <c r="C2446" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2447" spans="1:3" x14ac:dyDescent="0.2">
@@ -43126,7 +43123,7 @@
         <v>2447</v>
       </c>
       <c r="C2447" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2448" spans="1:3" x14ac:dyDescent="0.2">
@@ -43137,7 +43134,7 @@
         <v>2448</v>
       </c>
       <c r="C2448" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2449" spans="1:3" x14ac:dyDescent="0.2">
@@ -43148,7 +43145,7 @@
         <v>2449</v>
       </c>
       <c r="C2449" s="3">
-        <v>28692.09</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2450" spans="1:3" x14ac:dyDescent="0.2">
@@ -43159,7 +43156,7 @@
         <v>2450</v>
       </c>
       <c r="C2450" s="3">
-        <v>34088.85</v>
+        <v>27913.185000000001</v>
       </c>
     </row>
     <row r="2451" spans="1:3" x14ac:dyDescent="0.2">
@@ -58064,7 +58061,7 @@
         <v>3800</v>
       </c>
       <c r="C3805" s="3">
-        <v>25089.119999999999</v>
+        <v>26343.576000000001</v>
       </c>
     </row>
     <row r="3806" spans="1:3" x14ac:dyDescent="0.2">
@@ -58075,7 +58072,7 @@
         <v>3801</v>
       </c>
       <c r="C3806" s="3">
-        <v>42902.19</v>
+        <v>45047.299500000001</v>
       </c>
     </row>
     <row r="3807" spans="1:3" x14ac:dyDescent="0.2">
@@ -58086,7 +58083,7 @@
         <v>3802</v>
       </c>
       <c r="C3807" s="3">
-        <v>47122.47</v>
+        <v>49478.593500000003</v>
       </c>
     </row>
     <row r="3808" spans="1:3" x14ac:dyDescent="0.2">
@@ -58119,7 +58116,7 @@
         <v>3805</v>
       </c>
       <c r="C3810" s="3">
-        <v>26833.32</v>
+        <v>28174.986000000001</v>
       </c>
     </row>
     <row r="3811" spans="1:3" x14ac:dyDescent="0.2">
@@ -58130,7 +58127,7 @@
         <v>3806</v>
       </c>
       <c r="C3811" s="3">
-        <v>27357.435000000001</v>
+        <v>28725.30675</v>
       </c>
     </row>
     <row r="3812" spans="1:3" x14ac:dyDescent="0.2">
@@ -58141,7 +58138,7 @@
         <v>3807</v>
       </c>
       <c r="C3812" s="3">
-        <v>32661.855</v>
+        <v>34294.947749999999</v>
       </c>
     </row>
     <row r="3813" spans="1:3" x14ac:dyDescent="0.2">
@@ -58152,7 +58149,7 @@
         <v>3808</v>
       </c>
       <c r="C3813" s="3">
-        <v>33055.154999999999</v>
+        <v>34707.912750000003</v>
       </c>
     </row>
     <row r="3814" spans="1:3" x14ac:dyDescent="0.2">
@@ -58163,7 +58160,7 @@
         <v>3809</v>
       </c>
       <c r="C3814" s="3">
-        <v>34461.629999999997</v>
+        <v>36184.711499999998</v>
       </c>
     </row>
     <row r="3815" spans="1:3" x14ac:dyDescent="0.2">
@@ -58174,7 +58171,7 @@
         <v>3810</v>
       </c>
       <c r="C3815" s="3">
-        <v>35248.230000000003</v>
+        <v>37010.641499999998</v>
       </c>
     </row>
     <row r="3816" spans="1:3" x14ac:dyDescent="0.2">
@@ -70626,7 +70623,7 @@
         <v>4941</v>
       </c>
       <c r="C4947" s="3">
-        <v>0</v>
+        <v>81885.914999999994</v>
       </c>
     </row>
     <row r="4948" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
🔄 Actualización automática 2025-08-20 10:47:02
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\CotizadorKitchenTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{280E1017-A5FE-446A-8A1D-AADEBAEA777C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E151912-BBF5-4D30-B19C-728BFD8AAC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15C47D69-194B-4534-8153-D36587208E4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96443FD4-0DB6-4D1F-A888-BFE31970C3D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Precio" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -2438,7 +2425,7 @@
     <t>COCKTELERA AC. BOSTON 450/600 CC REFORZ. NEGRA</t>
   </si>
   <si>
-    <t>COCKTELERA AC. CLASICA 500 / 550 CC TAPA ALTA (29797)</t>
+    <t>COCKTELERA AC. CLASICA 500 / 550 CC TAPA ALTA (IN170044)</t>
   </si>
   <si>
     <t>COCKTELERA AC. CLASICA 500 / 550 CC TAPA ALTA- AZUL (IN180182-A)</t>
@@ -12686,7 +12673,7 @@
     <t>SET DE COCTELERIA BARMAN PELTRE</t>
   </si>
   <si>
-    <t>SET DE COCTELERIA COCTELERA BASE PLASTICA</t>
+    <t>SET DE COCTELERIA COCTELERA TAPA ALTA</t>
   </si>
   <si>
     <t>SET DE COCTELERIA GRANDE</t>
@@ -15797,11 +15784,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C339761-B461-42C2-9161-2C45454A5B8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9514B9D-FDF9-4547-B4D8-01D107D5AE1E}">
   <dimension ref="A1:C5125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5082" workbookViewId="0">
-      <selection activeCell="B5085" sqref="B5085"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>